<commit_message>
put a star on the graph
</commit_message>
<xml_diff>
--- a/images/resultsCoding.xlsx
+++ b/images/resultsCoding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="0" windowWidth="23480" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="1140" yWindow="0" windowWidth="23480" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -229,8 +229,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -303,9 +307,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -335,6 +339,8 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -364,6 +370,8 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -533,11 +541,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127800488"/>
-        <c:axId val="2128411256"/>
+        <c:axId val="2127984408"/>
+        <c:axId val="2122509336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127800488"/>
+        <c:axId val="2127984408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,7 +554,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128411256"/>
+        <c:crossAx val="2122509336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -554,7 +562,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2128411256"/>
+        <c:axId val="2122509336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -565,7 +573,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127800488"/>
+        <c:crossAx val="2127984408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -950,8 +958,8 @@
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>